<commit_message>
Pregunta 01 - finalizada
</commit_message>
<xml_diff>
--- a/2. CIRCUITOS RESONANTES/INFORME FINAL/resonancia.xlsx
+++ b/2. CIRCUITOS RESONANTES/INFORME FINAL/resonancia.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bremdows\UNSAAC\SEMESTRE VIII\CIRCUITOS ELECTRONICOS III\laboratorio\2. CIRCUITOS RESONANTES\INFORME FINAL\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UNSAAC\SEMESTRE VIII\CIRCUITOS ELECTRÓNICOS IIII\laboratorio\2. CIRCUITOS RESONANTES\INFORME FINAL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBA75251-5D17-489A-95F8-D51924F1E5B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA8A62A3-C825-476E-9336-D013799D7924}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1536" windowWidth="16140" windowHeight="11424" xr2:uid="{13B88763-F0A5-42E8-9ED8-A377EE544D25}"/>
+    <workbookView xWindow="810" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{13B88763-F0A5-42E8-9ED8-A377EE544D25}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -157,6 +157,1170 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Io [mA] -</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Frecuencia generador [Hz]</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-PE"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Hoja1!$F$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Io [mA]</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Hoja1!$D$3:$D$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>700</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>708.93</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>850</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>950</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1200</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2500</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>3500</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>5000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Hoja1!$F$2:$F$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.666875</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.0329999999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.325</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.391</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.409</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.4119999999999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.413</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.4139999999999999</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.4139999999999999</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.4139999999999999</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.4139999999999999</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.4139999999999999</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.4139999999999999</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.4139999999999999</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.4139999999999999</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1.411</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1.409</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1.403</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1.39</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-8C09-41D9-A3EA-176AD4D97913}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="803951311"/>
+        <c:axId val="803951791"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="803951311"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="es-PE"/>
+                  <a:t>Frecuencia</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="es-PE" baseline="0"/>
+                  <a:t> [Hz]</a:t>
+                </a:r>
+                <a:endParaRPr lang="es-PE"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="es-PE"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-PE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="803951791"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="803951791"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="es-PE"/>
+                  <a:t>Corriente Io</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="es-PE" baseline="0"/>
+                  <a:t> -{mA}</a:t>
+                </a:r>
+                <a:endParaRPr lang="es-PE"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="es-PE"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-PE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="803951311"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-PE"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>761999</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>190499</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>733424</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>142874</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Gráfico 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FFE5CACA-6CFA-EC08-0DE2-798BB4944A3B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -458,18 +1622,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9977AB2-8B64-4119-B5C3-5A5B692B16F2}">
   <dimension ref="A1:K21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="L31" sqref="L31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="14.21875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="14.28515625" style="2" customWidth="1"/>
     <col min="5" max="5" width="14" style="2" customWidth="1"/>
-    <col min="6" max="6" width="14.88671875" style="2" customWidth="1"/>
+    <col min="6" max="6" width="14.85546875" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
@@ -483,7 +1647,7 @@
       <c r="E1" s="5"/>
       <c r="F1" s="5"/>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
@@ -507,7 +1671,7 @@
       <c r="J2" s="6"/>
       <c r="K2" s="6"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>0</v>
       </c>
@@ -529,7 +1693,7 @@
       <c r="J3" s="6"/>
       <c r="K3" s="6"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
@@ -551,7 +1715,7 @@
       <c r="J4" s="6"/>
       <c r="K4" s="6"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D5" s="1">
         <v>50</v>
       </c>
@@ -566,7 +1730,7 @@
       <c r="J5" s="6"/>
       <c r="K5" s="6"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D6" s="1">
         <v>100</v>
       </c>
@@ -581,7 +1745,7 @@
       <c r="J6" s="6"/>
       <c r="K6" s="6"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D7" s="1">
         <f>D6 + 100</f>
         <v>200</v>
@@ -597,7 +1761,7 @@
       <c r="J7" s="6"/>
       <c r="K7" s="6"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D8" s="1">
         <f t="shared" ref="D8:D12" si="0">D7 + 100</f>
         <v>300</v>
@@ -613,7 +1777,7 @@
       <c r="J8" s="6"/>
       <c r="K8" s="6"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D9" s="1">
         <f t="shared" si="0"/>
         <v>400</v>
@@ -629,7 +1793,7 @@
       <c r="J9" s="6"/>
       <c r="K9" s="6"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D10" s="1">
         <f t="shared" si="0"/>
         <v>500</v>
@@ -645,7 +1809,7 @@
       <c r="J10" s="6"/>
       <c r="K10" s="6"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D11" s="1">
         <f t="shared" si="0"/>
         <v>600</v>
@@ -661,7 +1825,7 @@
       <c r="J11" s="6"/>
       <c r="K11" s="6"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D12" s="1">
         <f t="shared" si="0"/>
         <v>700</v>
@@ -677,7 +1841,7 @@
       <c r="J12" s="6"/>
       <c r="K12" s="6"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D13" s="1">
         <v>708.93</v>
       </c>
@@ -692,7 +1856,7 @@
       <c r="J13" s="6"/>
       <c r="K13" s="6"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D14" s="1">
         <v>850</v>
       </c>
@@ -707,7 +1871,7 @@
       <c r="J14" s="6"/>
       <c r="K14" s="6"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D15" s="1">
         <v>950</v>
       </c>
@@ -722,7 +1886,7 @@
       <c r="J15" s="6"/>
       <c r="K15" s="6"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D16" s="1">
         <v>1000</v>
       </c>
@@ -737,7 +1901,7 @@
       <c r="J16" s="6"/>
       <c r="K16" s="6"/>
     </row>
-    <row r="17" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D17" s="1">
         <v>1200</v>
       </c>
@@ -752,7 +1916,7 @@
       <c r="J17" s="6"/>
       <c r="K17" s="6"/>
     </row>
-    <row r="18" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D18" s="1">
         <v>2000</v>
       </c>
@@ -767,7 +1931,7 @@
       <c r="J18" s="6"/>
       <c r="K18" s="6"/>
     </row>
-    <row r="19" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D19" s="1">
         <v>2500</v>
       </c>
@@ -782,7 +1946,7 @@
       <c r="J19" s="6"/>
       <c r="K19" s="6"/>
     </row>
-    <row r="20" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="20" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D20" s="1">
         <v>3500</v>
       </c>
@@ -797,7 +1961,7 @@
       <c r="J20" s="6"/>
       <c r="K20" s="6"/>
     </row>
-    <row r="21" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="21" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D21" s="1">
         <v>5000</v>
       </c>
@@ -819,5 +1983,6 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>